<commit_message>
Cambios para el servidor
</commit_message>
<xml_diff>
--- a/storage/app/public/files/files_out/Centro_de_Costos_122_1.xlsx
+++ b/storage/app/public/files/files_out/Centro_de_Costos_122_1.xlsx
@@ -2340,7 +2340,7 @@
         <v>621</v>
       </c>
       <c r="D5" s="2">
-        <f>Recaudos_SAP!B84</f>
+        <f>Recaudos_SAP!B85</f>
         <v>0</v>
       </c>
       <c r="E5" s="2">
@@ -2394,7 +2394,7 @@
         <v>621</v>
       </c>
       <c r="D12" s="2">
-        <f>Pagos_SAP!B364</f>
+        <f>Pagos_SAP!B365</f>
         <v>0</v>
       </c>
       <c r="E12" s="2">

</xml_diff>